<commit_message>
set refinements to bnous
</commit_message>
<xml_diff>
--- a/hw3-review.xlsx
+++ b/hw3-review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsaleem/Documents/HU/Courses/2021_Spring/CS201/hw/hw3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886B1160-0BBE-E94C-A1FF-844638B55834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A900F2-1494-7E49-8B37-39D337CA6143}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,9 +117,6 @@
     <t>Meets 75% or more of the expectation .</t>
   </si>
   <si>
-    <t>awesome</t>
-  </si>
-  <si>
     <t>In the awesome branch, the refinements are adequately described in the README and correctly implemented. They represent insight, thought, and effort, ranging from (low:) case insensitivity to (medium:) stemming, stopword removal, or higher. Surprise us!</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Correctly returns a ranked list of documents in the index as per similarity with the wuery.</t>
+  </si>
+  <si>
+    <t>awesome (bonus)</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1195,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="14">
         <v>10</v>
@@ -1211,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="14">
         <v>10</v>
@@ -1227,7 +1229,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="14">
         <v>5</v>
@@ -1243,7 +1245,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14">
         <v>10</v>
@@ -1259,7 +1261,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="14">
         <v>20</v>
@@ -1286,10 +1288,10 @@
     </row>
     <row r="12" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="C12" s="14">
         <v>10</v>
@@ -1352,7 +1354,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="16">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D16" s="11">
         <f>SUMPRODUCT(C3:C15,D3:D15)</f>

</xml_diff>